<commit_message>
add: shift reg 74HC165 driver
</commit_message>
<xml_diff>
--- a/Docs/ModBus.xlsx
+++ b/Docs/ModBus.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="211">
   <si>
     <t xml:space="preserve">Номер</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Количество обнаруженных приводов</t>
   </si>
   <si>
-    <t xml:space="preserve">5-127</t>
+    <t xml:space="preserve">5-63</t>
   </si>
   <si>
     <t xml:space="preserve">--</t>
@@ -79,31 +79,31 @@
     <t xml:space="preserve">Зарезервировано</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 0</t>
+    <t xml:space="preserve">(Id * 64) + 0</t>
   </si>
   <si>
     <t xml:space="preserve">Firmware servo major version</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 1</t>
+    <t xml:space="preserve">(Id * 64) + 1</t>
   </si>
   <si>
     <t xml:space="preserve">Firmware servo minor version</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 2</t>
+    <t xml:space="preserve">(Id * 64) + 2</t>
   </si>
   <si>
     <t xml:space="preserve">Servo major version</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 3</t>
+    <t xml:space="preserve">(Id * 64) + 3</t>
   </si>
   <si>
     <t xml:space="preserve">Servo minor version</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 4</t>
+    <t xml:space="preserve">(Id * 64) + 4</t>
   </si>
   <si>
     <t xml:space="preserve">Actual position</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">шаг</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 5</t>
+    <t xml:space="preserve">(Id * 64) + 5</t>
   </si>
   <si>
     <t xml:space="preserve">Actual speed</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">шаг/сек</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 6</t>
+    <t xml:space="preserve">(Id * 64) + 6</t>
   </si>
   <si>
     <t xml:space="preserve">Actual load</t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">%</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 7</t>
+    <t xml:space="preserve">(Id * 64) + 7</t>
   </si>
   <si>
     <t xml:space="preserve">Actual voltage</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">В</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 8</t>
+    <t xml:space="preserve">(Id * 64) + 8</t>
   </si>
   <si>
     <t xml:space="preserve">Actual temperature</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Град</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 9</t>
+    <t xml:space="preserve">(Id * 64) + 9</t>
   </si>
   <si>
     <t xml:space="preserve">Servo status</t>
@@ -162,7 +162,7 @@
 Bit 5 overload </t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 10</t>
+    <t xml:space="preserve">(Id * 64) + 10</t>
   </si>
   <si>
     <t xml:space="preserve">Actual current</t>
@@ -448,7 +448,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">22 — 127</t>
+    <t xml:space="preserve">22 — 63</t>
   </si>
   <si>
     <t xml:space="preserve">---</t>
@@ -515,31 +515,31 @@
     <t xml:space="preserve">Unloading condition</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 11</t>
+    <t xml:space="preserve">(Id * 64) + 11</t>
   </si>
   <si>
     <t xml:space="preserve">LED Alarm condition</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 12</t>
+    <t xml:space="preserve">(Id * 64) + 12</t>
   </si>
   <si>
     <t xml:space="preserve">P Proportionality coefficient</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 13</t>
+    <t xml:space="preserve">(Id * 64) + 13</t>
   </si>
   <si>
     <t xml:space="preserve">D Differential coefficient</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 14</t>
+    <t xml:space="preserve">(Id * 64) + 14</t>
   </si>
   <si>
     <t xml:space="preserve">I Integral coefficient</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 15</t>
+    <t xml:space="preserve">(Id * 64) + 15</t>
   </si>
   <si>
     <t xml:space="preserve">Minimum startup force</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">0-100</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 16</t>
+    <t xml:space="preserve">(Id * 64) + 16</t>
   </si>
   <si>
     <t xml:space="preserve">Clockwise insensitive area</t>
@@ -557,13 +557,13 @@
     <t xml:space="preserve">0-32</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 17</t>
+    <t xml:space="preserve">(Id * 64) + 17</t>
   </si>
   <si>
     <t xml:space="preserve">Counterclockwise insensitive region</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 18</t>
+    <t xml:space="preserve">(Id * 64) + 18</t>
   </si>
   <si>
     <t xml:space="preserve">Protection current</t>
@@ -572,7 +572,7 @@
     <t xml:space="preserve">0-3,255</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 19</t>
+    <t xml:space="preserve">(Id * 64) + 19</t>
   </si>
   <si>
     <t xml:space="preserve">Angular resolution</t>
@@ -581,13 +581,13 @@
     <t xml:space="preserve">1-100</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 20</t>
+    <t xml:space="preserve">(Id * 64) + 20</t>
   </si>
   <si>
     <t xml:space="preserve">Position correction</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 21</t>
+    <t xml:space="preserve">(Id * 64) + 21</t>
   </si>
   <si>
     <t xml:space="preserve">Operation mode</t>
@@ -602,13 +602,13 @@
 3: Управление по шагу. Управляется [HoldRegs 42], где параметром задается сколько шагов нужно сделать</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 22</t>
+    <t xml:space="preserve">(Id * 64) + 22</t>
   </si>
   <si>
     <t xml:space="preserve">Protective torque</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 23</t>
+    <t xml:space="preserve">(Id * 64) + 23</t>
   </si>
   <si>
     <t xml:space="preserve">Protection time</t>
@@ -617,31 +617,31 @@
     <t xml:space="preserve">мс</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 24</t>
+    <t xml:space="preserve">(Id * 64) + 24</t>
   </si>
   <si>
     <t xml:space="preserve">Overload torque</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 25</t>
+    <t xml:space="preserve">(Id * 64) + 25</t>
   </si>
   <si>
     <t xml:space="preserve">Speed closed loop P proportional coefficient</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 26</t>
+    <t xml:space="preserve">(Id * 64) + 26</t>
   </si>
   <si>
     <t xml:space="preserve">Over current protection time</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 27</t>
+    <t xml:space="preserve">(Id * 64) + 27</t>
   </si>
   <si>
     <t xml:space="preserve">Velocity closed loop I integral coefficient</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 28</t>
+    <t xml:space="preserve">(Id * 64) + 28</t>
   </si>
   <si>
     <t xml:space="preserve">Torque switch</t>
@@ -655,7 +655,7 @@
 128: current position correction is 2048</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 29</t>
+    <t xml:space="preserve">(Id * 64) + 29</t>
   </si>
   <si>
     <t xml:space="preserve">Acceleration</t>
@@ -664,7 +664,7 @@
     <t xml:space="preserve">шаг/с^2</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 30</t>
+    <t xml:space="preserve">(Id * 64) + 30</t>
   </si>
   <si>
     <t xml:space="preserve">Target position</t>
@@ -673,19 +673,19 @@
     <t xml:space="preserve">Задается или абсолютное положение, или относительное, в зависимости от режима управления</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 31</t>
+    <t xml:space="preserve">(Id * 64) + 31</t>
   </si>
   <si>
     <t xml:space="preserve">Target duty</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 32</t>
+    <t xml:space="preserve">(Id * 64) + 32</t>
   </si>
   <si>
     <t xml:space="preserve">Target speed</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id * 128) + 33</t>
+    <t xml:space="preserve">(Id * 64) + 33</t>
   </si>
   <si>
     <t xml:space="preserve">Torque limit</t>
@@ -694,29 +694,112 @@
     <t xml:space="preserve">0 — 1000 </t>
   </si>
   <si>
-    <t xml:space="preserve">…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Id * 128) + 51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activate SW 1</t>
+    <t xml:space="preserve">(ID * 64) + 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 1 Num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номер датчка 1, ассоциированного с сервоприводом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 2 Num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номер датчка 2, ассоциированного с сервоприводом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 3 Num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номер датчка 3, ассоциированного с сервоприводом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 4 Num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Номер датчка 4, ассоциированного с сервоприводом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 1 Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-2</t>
   </si>
   <si>
     <t xml:space="preserve">Действие при срабатывании концевого датчика 1:
 0: Нет действия
-1: Остановка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Id * 128) + 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activate SW 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Действие при срабатывании концевого датчика 50: 
+1: Остановка
+2: Замедление</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 2 Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Действие при срабатывании концевого датчика 2:
+0: Нет действия
+1: Остановка
+2: Замедление</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 3 Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Действие при срабатывании концевого датчика 3: 
 0: Нет действия 
-1: Остановка</t>
+1: Остановка
+2: Замедление</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 4 Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Действие при срабатывании концевого датчика 4: 
+0: Нет действия 
+1: Остановка
+2: Замедление</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slowdown Deacc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Интенсивность замедления в функции «Замедление»</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slowdown Speed Lim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Целевая скорость замедления в функции «Замедление»</t>
   </si>
   <si>
     <t xml:space="preserve">0 — 49</t>
@@ -728,10 +811,10 @@
     <t xml:space="preserve">Состояние концевиков</t>
   </si>
   <si>
-    <t xml:space="preserve">51 — 127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(ID * 128) + 0</t>
+    <t xml:space="preserve">51 — 63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ID * 64) + 0</t>
   </si>
   <si>
     <t xml:space="preserve">Servo is online</t>
@@ -740,7 +823,7 @@
     <t xml:space="preserve">привод в сети</t>
   </si>
   <si>
-    <t xml:space="preserve">(ID * 128) + 1</t>
+    <t xml:space="preserve">(ID * 64) + 1</t>
   </si>
   <si>
     <t xml:space="preserve">Servo is moving</t>
@@ -749,7 +832,39 @@
     <t xml:space="preserve">привод в движении</t>
   </si>
   <si>
-    <t xml:space="preserve">0-127</t>
+    <t xml:space="preserve">SW 1 Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус концевика 1
+0: неактивен,
+1: активен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 2 Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус концевика 2
+0: неактивен,
+1: активен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 3 Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус концевика 3
+0: неактивен,
+1: активен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 4 Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус концевика 4
+0: неактивен,
+1: активен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-63</t>
   </si>
   <si>
     <t xml:space="preserve">Response status level</t>
@@ -894,7 +1009,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -991,6 +1106,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1072,10 +1191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1330,6 +1449,26 @@
         <v>46</v>
       </c>
       <c r="E18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="E19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="E20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="E21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+      <c r="E22" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1347,10 +1486,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2230,66 +2369,190 @@
       <c r="F52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="14" t="s">
+      <c r="B53" s="14" t="s">
         <v>158</v>
       </c>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="F53" s="24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="24" t="s">
+        <v>161</v>
+      </c>
       <c r="B54" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="16" t="s">
-        <v>160</v>
+      <c r="F54" s="24" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14" t="s">
-        <v>157</v>
+      <c r="A55" s="24" t="s">
+        <v>164</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-    </row>
-    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="14" t="s">
-        <v>161</v>
+        <v>165</v>
+      </c>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="F55" s="24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="24" t="s">
+        <v>167</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="16" t="s">
-        <v>163</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F58" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F59" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="F60" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61" s="24" t="n">
+        <v>100</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="C62" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0"/>
+      <c r="B63" s="0"/>
+      <c r="E63" s="0"/>
+      <c r="F63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0"/>
+      <c r="B64" s="0"/>
+      <c r="E64" s="0"/>
+      <c r="F64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0"/>
+      <c r="B65" s="0"/>
+      <c r="E65" s="0"/>
+      <c r="F65" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2307,10 +2570,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2338,20 +2601,20 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -2368,28 +2631,80 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>173</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="8" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2411,7 +2726,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2440,7 +2755,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -2457,10 +2772,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>175</v>
+        <v>193</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -2468,15 +2783,15 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add end switches handlers
</commit_message>
<xml_diff>
--- a/Docs/ModBus.xlsx
+++ b/Docs/ModBus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="InputRegs" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="213">
   <si>
     <t xml:space="preserve">Номер</t>
   </si>
@@ -864,7 +864,13 @@
 1: активен</t>
   </si>
   <si>
-    <t xml:space="preserve">0-63</t>
+    <t xml:space="preserve">Save Cfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сохранить настройки устройства во FLASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-63</t>
   </si>
   <si>
     <t xml:space="preserve">Response status level</t>
@@ -1106,7 +1112,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1191,10 +1197,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1449,26 +1455,6 @@
         <v>46</v>
       </c>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-      <c r="E19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-      <c r="E20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="E21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="B22" s="0"/>
-      <c r="E22" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1486,9 +1472,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2369,71 +2355,71 @@
       <c r="F52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="14" t="s">
         <v>157</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24" t="s">
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="F53" s="24" t="s">
+      <c r="F53" s="14" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="24" t="s">
+      <c r="A54" s="14" t="s">
         <v>161</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24" t="s">
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="F54" s="24" t="s">
+      <c r="F54" s="14" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="14" t="s">
         <v>164</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24" t="s">
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="F55" s="24" t="s">
+      <c r="F55" s="14" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="14" t="s">
         <v>167</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24" t="s">
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="F56" s="24" t="s">
+      <c r="F56" s="14" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="14" t="s">
         <v>170</v>
       </c>
       <c r="B57" s="14" t="s">
@@ -2449,7 +2435,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="14" t="s">
         <v>174</v>
       </c>
       <c r="B58" s="14" t="s">
@@ -2465,7 +2451,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="24" t="s">
+      <c r="A59" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B59" s="14" t="s">
@@ -2481,7 +2467,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B60" s="14" t="s">
@@ -2497,13 +2483,13 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B61" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C61" s="24" t="n">
+      <c r="C61" s="14" t="n">
         <v>100</v>
       </c>
       <c r="D61" s="14" t="s">
@@ -2512,18 +2498,18 @@
       <c r="E61" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F61" s="24" t="s">
+      <c r="F61" s="14" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C62" s="24" t="n">
+      <c r="C62" s="14" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="14" t="s">
@@ -2532,27 +2518,9 @@
       <c r="E62" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F62" s="24" t="s">
+      <c r="F62" s="14" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0"/>
-      <c r="B63" s="0"/>
-      <c r="E63" s="0"/>
-      <c r="F63" s="0"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0"/>
-      <c r="B64" s="0"/>
-      <c r="E64" s="0"/>
-      <c r="F64" s="0"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0"/>
-      <c r="B65" s="0"/>
-      <c r="E65" s="0"/>
-      <c r="F65" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2723,10 +2691,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2754,44 +2722,57 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>209</v>
+      <c r="B4" s="25" t="s">
+        <v>210</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>210</v>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>